<commit_message>
script for import cards
</commit_message>
<xml_diff>
--- a/Assets/Cards/Cards.xlsx
+++ b/Assets/Cards/Cards.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="154">
   <si>
     <t>Сорока-мать</t>
   </si>
@@ -126,7 +126,7 @@
     <t>Сорока-ворчунья</t>
   </si>
   <si>
-    <t>редакая</t>
+    <t>редкая</t>
   </si>
   <si>
     <t>Заблокируйте две любые клетки</t>
@@ -138,9 +138,6 @@
     <t>Сорока-вор</t>
   </si>
   <si>
-    <t>редкая</t>
-  </si>
-  <si>
     <t>Вы крадете карту из руки противника и уничтожаете ее</t>
   </si>
   <si>
@@ -186,9 +183,6 @@
     <t>Возьмите карту и уничтожьте соседнюю свободную клетку</t>
   </si>
   <si>
-    <t>Free Select Magpie Spawn Free Adjacent Select Destroy Draw</t>
-  </si>
-  <si>
     <t>Сорока-верующая</t>
   </si>
   <si>
@@ -246,7 +240,7 @@
     <t>Free Select Beaver Spawn NExisting Select Build Beaver Spawn NExisting Select Build Beaver Spawn NExisting Select Build Beaver Spawn</t>
   </si>
   <si>
-    <t>Бобёр-шахтер</t>
+    <t>Бобёр-шахтёр</t>
   </si>
   <si>
     <t>Постройте клетку и поставьте на нее бобра</t>
@@ -264,7 +258,7 @@
     <t>Free Select ShiftAnchor Beaver Spawn Adjacent Beaver Occupied Select Push</t>
   </si>
   <si>
-    <t>Бобренок</t>
+    <t>Бобрёнок</t>
   </si>
   <si>
     <t>Free Select Beaver Spawn</t>
@@ -1106,10 +1100,10 @@
         <v>40</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="D15" s="11">
         <v>13.0</v>
@@ -1117,129 +1111,148 @@
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="D16" s="2">
         <v>14.0</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="D17" s="2">
         <v>15.0</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="D18" s="2">
         <v>16.0</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="D19" s="2">
         <v>17.0</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="D20" s="2">
         <v>18.0</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="E20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D21" s="5">
         <v>19.0</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="D22" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>63</v>
-      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+      <c r="Z22" s="6"/>
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D23" s="5">
         <v>21.0</v>
@@ -1247,13 +1260,13 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D24" s="5">
         <v>22.0</v>
@@ -1261,36 +1274,36 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D25" s="2">
         <v>23.0</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D26" s="2">
         <v>24.0</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1322,58 +1335,58 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D2" s="2">
         <v>25.0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D3" s="2">
         <v>26.0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D4" s="2">
         <v>27.0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -1383,12 +1396,12 @@
         <v>28.0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -1400,137 +1413,137 @@
         <v>29.0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D7" s="2">
         <v>30.0</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D8" s="2">
         <v>31.0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D9" s="2">
         <v>32.0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D10" s="2">
         <v>33.0</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D11" s="5">
         <v>34.0</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D12" s="2">
         <v>35.0</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D13" s="5">
         <v>36.0</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D14" s="11">
         <v>37.0</v>
@@ -1560,13 +1573,13 @@
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D15" s="5">
         <v>38.0</v>
@@ -1575,98 +1588,98 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D16" s="2">
         <v>39.0</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D17" s="2">
         <v>40.0</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D18" s="2">
         <v>41.0</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D19" s="2">
         <v>42.0</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D20" s="2">
         <v>43.0</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D21" s="18">
         <v>44.0</v>
@@ -1696,13 +1709,13 @@
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D22" s="5">
         <v>45.0</v>
@@ -1710,13 +1723,13 @@
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D23" s="11">
         <v>46.0</v>
@@ -1724,47 +1737,47 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D24" s="2">
         <v>47.0</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D25" s="2">
         <v>48.0</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D26" s="5">
         <v>49.0</v>
@@ -1793,51 +1806,51 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" ht="124.5" customHeight="1">
       <c r="A2" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="L2" s="20" t="s">
         <v>146</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B5" s="2">
         <v>6.0</v>
@@ -1845,7 +1858,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B6" s="2">
         <v>3.0</v>
@@ -1853,7 +1866,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B7" s="2">
         <v>1.0</v>

</xml_diff>

<commit_message>
new keywords TEMP & AWAIT
</commit_message>
<xml_diff>
--- a/Assets/Cards/Cards.xlsx
+++ b/Assets/Cards/Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\LuckyThicket\Assets\Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C37E815-467C-44DA-B462-DB5FF299C54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D42C6C-7FBD-4635-AB8B-8EEF73774A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -360,9 +360,6 @@
     <t>Ожидайте двух бобров на смежных клетках.</t>
   </si>
   <si>
-    <t>Создайте двух временных бобров на смежных клетках.</t>
-  </si>
-  <si>
     <t>Ожидайте сорочонка на случайной клетке.</t>
   </si>
   <si>
@@ -523,6 +520,9 @@
   </si>
   <si>
     <t>Создайте бобра на краю поля и уничтожьте сороку на краю поля.</t>
+  </si>
+  <si>
+    <t>Создайте двух бобров на смежных клетках. На следующем ходу отряды в этих клетках погибнут.</t>
   </si>
 </sst>
 </file>
@@ -935,7 +935,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D2" s="11">
         <v>0</v>
@@ -952,7 +952,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" s="11">
         <v>1</v>
@@ -969,7 +969,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D4" s="11">
         <v>2</v>
@@ -986,13 +986,13 @@
         <v>4</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D5" s="11">
         <v>3</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1018,7 +1018,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D7" s="11">
         <v>5</v>
@@ -1035,7 +1035,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D8" s="11">
         <v>6</v>
@@ -1052,13 +1052,13 @@
         <v>4</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D9" s="11">
         <v>7</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1069,7 +1069,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D10" s="11">
         <v>8</v>
@@ -1086,7 +1086,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D11" s="11">
         <v>9</v>
@@ -1103,13 +1103,13 @@
         <v>4</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D12" s="11">
         <v>10</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1120,7 +1120,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D13" s="11">
         <v>11</v>
@@ -1137,7 +1137,7 @@
         <v>20</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D14" s="11">
         <v>12</v>
@@ -1154,7 +1154,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D15" s="11">
         <v>13</v>
@@ -1171,7 +1171,7 @@
         <v>20</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D16" s="11">
         <v>14</v>
@@ -1188,7 +1188,7 @@
         <v>20</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D17" s="11">
         <v>15</v>
@@ -1205,7 +1205,7 @@
         <v>20</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D18" s="11">
         <v>16</v>
@@ -1222,7 +1222,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D19" s="11">
         <v>17</v>
@@ -1239,13 +1239,13 @@
         <v>20</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D20" s="11">
         <v>18</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
@@ -1256,13 +1256,13 @@
         <v>20</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D21" s="11">
         <v>19</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
@@ -1273,13 +1273,13 @@
         <v>34</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D22" s="11">
         <v>20</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -1311,7 +1311,7 @@
         <v>34</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D23" s="11">
         <v>21</v>
@@ -1328,13 +1328,13 @@
         <v>34</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D24" s="11">
         <v>22</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1345,7 +1345,7 @@
         <v>34</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D25" s="11">
         <v>23</v>
@@ -1362,13 +1362,13 @@
         <v>34</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D26" s="11">
         <v>24</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1388,7 +1388,7 @@
   <dimension ref="A1:Z26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1416,7 +1416,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D2" s="11">
         <v>25</v>
@@ -1433,7 +1433,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D3" s="11">
         <v>26</v>
@@ -1450,7 +1450,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D4" s="11">
         <v>27</v>
@@ -1482,13 +1482,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D6" s="11">
         <v>29</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
@@ -1499,7 +1499,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D7" s="11">
         <v>30</v>
@@ -1516,7 +1516,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D8" s="11">
         <v>31</v>
@@ -1533,7 +1533,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D9" s="11">
         <v>32</v>
@@ -1550,7 +1550,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D10" s="11">
         <v>33</v>
@@ -1567,13 +1567,13 @@
         <v>4</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D11" s="14">
         <v>34</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
@@ -1584,7 +1584,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D12" s="11">
         <v>35</v>
@@ -1601,13 +1601,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D13" s="14">
         <v>36</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1618,7 +1618,7 @@
         <v>20</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D14" s="20">
         <v>37</v>
@@ -1656,7 +1656,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>108</v>
+        <v>162</v>
       </c>
       <c r="D15" s="14">
         <v>38</v>
@@ -1673,7 +1673,7 @@
         <v>20</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D16" s="11">
         <v>39</v>
@@ -1690,7 +1690,7 @@
         <v>20</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D17" s="11">
         <v>40</v>
@@ -1707,13 +1707,13 @@
         <v>20</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D18" s="11">
         <v>41</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
@@ -1724,7 +1724,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D19" s="11">
         <v>42</v>
@@ -1741,7 +1741,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D20" s="11">
         <v>43</v>
@@ -1758,13 +1758,13 @@
         <v>20</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D21" s="25">
         <v>44</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -1796,7 +1796,7 @@
         <v>34</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D22" s="14">
         <v>45</v>
@@ -1830,7 +1830,7 @@
         <v>34</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D24" s="11">
         <v>47</v>
@@ -1847,7 +1847,7 @@
         <v>34</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D25" s="11">
         <v>48</v>

</xml_diff>

<commit_message>
started working on a new engine
</commit_message>
<xml_diff>
--- a/Assets/Cards/Cards.xlsx
+++ b/Assets/Cards/Cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BBproj\LuckyThicket\Assets\Cards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\LuckyThicket\Assets\Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045877F7-EA34-4FAD-A02B-AA3D5DF50AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC782A1-9BE0-45B6-944A-8D5DE366CC2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Magpies" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>обычная</t>
   </si>
   <si>
-    <t>Free Select Magpie Spawn Random Destroy</t>
-  </si>
-  <si>
     <t>Сорока-акушер</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>Сорока-иллюзионист</t>
   </si>
   <si>
-    <t>Free Select Magpie Spawn Free Surrounding Random Magpie Spawn</t>
-  </si>
-  <si>
     <t>Сорока-мастерица</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
     <t>Сорока-ниндзя</t>
   </si>
   <si>
-    <t>Free Select Magpie Spawn Beaver Occupied Random Kill Beaver Occupied Random Kill</t>
-  </si>
-  <si>
     <t>Сорока-вестница</t>
   </si>
   <si>
@@ -180,9 +171,6 @@
     <t>Бобёр-волшебник</t>
   </si>
   <si>
-    <t>Free Select Beaver Spawn Random Beaver Spawn</t>
-  </si>
-  <si>
     <t>Бобёр-дуболом</t>
   </si>
   <si>
@@ -232,9 +220,6 @@
   </si>
   <si>
     <t>Бобёр-камикадзе</t>
-  </si>
-  <si>
-    <t>Free Select Beaver Spawn Beaver Occupied Random Kill Magpie Occupied Select Kill Magpie Occupied Select Kill</t>
   </si>
   <si>
     <t>Бобёр-бродяга</t>
@@ -306,18 +291,12 @@
     <t>Free Select Magpie Spawn Obstacle Occupied Select Unlock</t>
   </si>
   <si>
-    <t>Free Select Magpie Spawn Free Random Await Magpie Spawn</t>
-  </si>
-  <si>
     <t>Free Select Beaver Spawn Adjacent Free Select Await Beaver Spawn Adjacent Free Select Await Beaver Spawn</t>
   </si>
   <si>
     <t>Free Select Beaver Spawn Playable Occupied Select ShiftAnchor NExisting Select Build Drag</t>
   </si>
   <si>
-    <t>Free Select Beaver Spawn Adjacent Free Select Temp Beaver Spawn Adjacent Free Select Temp Beaver Spawn</t>
-  </si>
-  <si>
     <t>Free Select Magpie Spawn Opponent Hand Discard</t>
   </si>
   <si>
@@ -516,24 +495,61 @@
     <t>Free Select Magpie Spawn Magpie Occupied Select ShiftAnchor Adjacent Free Select Drag ShiftAnchor Adjacent Free Select Drag</t>
   </si>
   <si>
-    <t xml:space="preserve">Free Select Magpie Spawn Beaver Occupied Adjacent Select Kill Also NExisting Random Build </t>
-  </si>
-  <si>
     <t>Уничтожьте бобра по соседству и постройте клетку в случайном месте.</t>
   </si>
   <si>
     <t>Free Select Beaver Spawn Completed Zero Playable Occupied Inc Inc Convert</t>
+  </si>
+  <si>
+    <t>Free Select Beaver Spawn Inc Beaver Spawn</t>
+  </si>
+  <si>
+    <t>Free Select Beaver Spawn Adjacent Free Select Beaver Spawn Temp Kill Adjacent Free Select Beaver Spawn Temp Kill</t>
+  </si>
+  <si>
+    <t>Free Select Beaver Spawn Beaver Occupied Inc Kill Magpie Occupied Select Kill Magpie Occupied Select Kill</t>
+  </si>
+  <si>
+    <t>Free Select Magpie Spawn Inc Destroy</t>
+  </si>
+  <si>
+    <t>Free Select Magpie Spawn Beaver Occupied Inc Inc Kill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free Select Magpie Spawn Beaver Occupied Adjacent Select Kill Also NExisting Inc Build </t>
+  </si>
+  <si>
+    <t>Free Select Magpie Spawn Free Await Magpie Inc Spawn</t>
+  </si>
+  <si>
+    <t>Free Select Magpie Spawn Free Surrounding Magpie Inc Spawn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -683,47 +699,50 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -945,25 +964,25 @@
   </sheetPr>
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.08984375" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
     <col min="3" max="3" width="75" customWidth="1"/>
-    <col min="5" max="5" width="99.36328125" customWidth="1"/>
+    <col min="5" max="5" width="118.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -971,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D2" s="11">
         <v>0</v>
@@ -980,7 +999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
@@ -988,334 +1007,334 @@
         <v>4</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D3" s="11">
         <v>1</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
-        <v>6</v>
-      </c>
       <c r="B4" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D4" s="11">
         <v>2</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="34" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D5" s="11">
         <v>3</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="11">
+        <v>4</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="11">
-        <v>4</v>
-      </c>
-      <c r="E6" s="11" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
-        <v>10</v>
-      </c>
       <c r="B7" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D7" s="11">
         <v>5</v>
       </c>
       <c r="E7" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
-        <v>12</v>
-      </c>
       <c r="B8" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D8" s="11">
         <v>6</v>
       </c>
       <c r="E8" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>14</v>
-      </c>
       <c r="B9" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D9" s="11">
         <v>7</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>15</v>
+      <c r="E9" s="32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D10" s="11">
         <v>8</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D11" s="11">
         <v>9</v>
       </c>
       <c r="E11" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>18</v>
-      </c>
       <c r="B12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="28" t="s">
-        <v>127</v>
+      <c r="C12" s="27" t="s">
+        <v>120</v>
       </c>
       <c r="D12" s="11">
         <v>10</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="28" t="s">
-        <v>128</v>
+      <c r="C13" s="27" t="s">
+        <v>121</v>
       </c>
       <c r="D13" s="11">
         <v>11</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>129</v>
+      <c r="C14" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="D14" s="11">
         <v>12</v>
       </c>
       <c r="E14" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>130</v>
+      <c r="B15" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>123</v>
       </c>
       <c r="D15" s="11">
         <v>13</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D16" s="11">
         <v>14</v>
       </c>
       <c r="E16" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
-        <v>25</v>
-      </c>
       <c r="B17" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D17" s="11">
         <v>15</v>
       </c>
-      <c r="E17" s="30" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>133</v>
+        <v>19</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>126</v>
       </c>
       <c r="D18" s="11">
         <v>16</v>
       </c>
-      <c r="E18" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="35" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>161</v>
+        <v>19</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>153</v>
       </c>
       <c r="D19" s="11">
         <v>17</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="32" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>134</v>
+        <v>19</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>127</v>
       </c>
       <c r="D20" s="11">
         <v>18</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D21" s="11">
         <v>19</v>
       </c>
-      <c r="E21" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>123</v>
+      <c r="C22" s="26" t="s">
+        <v>116</v>
       </c>
       <c r="D22" s="11">
         <v>20</v>
       </c>
-      <c r="E22" s="28" t="s">
-        <v>124</v>
+      <c r="E22" s="32" t="s">
+        <v>117</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -1339,72 +1358,72 @@
       <c r="Y22" s="6"/>
       <c r="Z22" s="6"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>135</v>
+        <v>30</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>128</v>
       </c>
       <c r="D23" s="11">
         <v>21</v>
       </c>
       <c r="E23" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
-        <v>35</v>
-      </c>
       <c r="B24" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D24" s="11">
         <v>22</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>137</v>
+        <v>30</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>130</v>
       </c>
       <c r="D25" s="11">
         <v>23</v>
       </c>
-      <c r="E25" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="32" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>138</v>
+        <v>30</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>131</v>
       </c>
       <c r="D26" s="11">
         <v>24</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1423,244 +1442,244 @@
   </sheetPr>
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.453125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" style="8"/>
-    <col min="3" max="3" width="80.6328125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" style="8"/>
-    <col min="5" max="5" width="108.08984375" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="12.6328125" style="8"/>
+    <col min="1" max="1" width="19.44140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="8"/>
+    <col min="3" max="3" width="80.6640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="8"/>
+    <col min="5" max="5" width="108.109375" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="12.6640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
     </row>
-    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="28" t="s">
-        <v>139</v>
+      <c r="C2" s="27" t="s">
+        <v>132</v>
       </c>
       <c r="D2" s="11">
         <v>25</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="28" t="s">
-        <v>140</v>
+      <c r="C3" s="27" t="s">
+        <v>133</v>
       </c>
       <c r="D3" s="11">
         <v>26</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D4" s="11">
         <v>27</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="11">
         <v>28</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="28" t="s">
-        <v>109</v>
+      <c r="C6" s="27" t="s">
+        <v>102</v>
       </c>
       <c r="D6" s="11">
         <v>29</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="28" t="s">
-        <v>141</v>
+      <c r="C7" s="27" t="s">
+        <v>134</v>
       </c>
       <c r="D7" s="11">
         <v>30</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="28" t="s">
-        <v>142</v>
+      <c r="C8" s="27" t="s">
+        <v>135</v>
       </c>
       <c r="D8" s="11">
         <v>31</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="28" t="s">
-        <v>143</v>
+      <c r="C9" s="27" t="s">
+        <v>136</v>
       </c>
       <c r="D9" s="11">
         <v>32</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+      <c r="E9" s="32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="28" t="s">
-        <v>107</v>
+      <c r="C10" s="27" t="s">
+        <v>100</v>
       </c>
       <c r="D10" s="11">
         <v>33</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="27" t="s">
-        <v>130</v>
+      <c r="C11" s="26" t="s">
+        <v>123</v>
       </c>
       <c r="D11" s="14">
         <v>34</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="28" t="s">
-        <v>144</v>
+      <c r="C12" s="27" t="s">
+        <v>137</v>
       </c>
       <c r="D12" s="11">
         <v>35</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>145</v>
+      <c r="C13" s="26" t="s">
+        <v>138</v>
       </c>
       <c r="D13" s="14">
         <v>36</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="D14" s="20">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D14" s="19">
         <v>37</v>
       </c>
-      <c r="E14" s="24" t="s">
-        <v>92</v>
+      <c r="E14" s="23" t="s">
+        <v>86</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="7"/>
@@ -1684,123 +1703,123 @@
       <c r="Y14" s="7"/>
       <c r="Z14" s="7"/>
     </row>
-    <row r="15" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="D15" s="14">
         <v>38</v>
       </c>
-      <c r="E15" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+      <c r="E15" s="33" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>147</v>
+        <v>19</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>140</v>
       </c>
       <c r="D16" s="11">
         <v>39</v>
       </c>
-      <c r="E16" s="29" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+      <c r="E16" s="28" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>148</v>
+        <v>19</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>141</v>
       </c>
       <c r="D17" s="11">
         <v>40</v>
       </c>
-      <c r="E17" s="29" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+      <c r="E17" s="28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>149</v>
+        <v>19</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>142</v>
       </c>
       <c r="D18" s="11">
         <v>41</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>150</v>
+        <v>19</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>143</v>
       </c>
       <c r="D19" s="11">
         <v>42</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>151</v>
+        <v>19</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>144</v>
       </c>
       <c r="D20" s="11">
         <v>43</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" ht="14" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="D21" s="25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" s="24">
         <v>44</v>
       </c>
-      <c r="E21" s="26" t="s">
-        <v>122</v>
+      <c r="E21" s="25" t="s">
+        <v>115</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -1824,89 +1843,89 @@
       <c r="Y21" s="7"/>
       <c r="Z21" s="7"/>
     </row>
-    <row r="22" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D22" s="14">
         <v>45</v>
       </c>
-      <c r="E22" s="32" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+      <c r="E22" s="31" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="20">
+        <v>64</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="19">
         <v>46</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>154</v>
+        <v>30</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>147</v>
       </c>
       <c r="D24" s="11">
         <v>47</v>
       </c>
-      <c r="E24" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+      <c r="E24" s="32" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>155</v>
+        <v>30</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>148</v>
       </c>
       <c r="D25" s="11">
         <v>48</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D26" s="14">
         <v>49</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1923,77 +1942,77 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.08984375" customWidth="1"/>
-    <col min="6" max="6" width="56.81640625" customWidth="1"/>
+    <col min="1" max="1" width="52.109375" customWidth="1"/>
+    <col min="6" max="6" width="56.77734375" customWidth="1"/>
     <col min="9" max="9" width="57" customWidth="1"/>
-    <col min="12" max="12" width="70.6328125" customWidth="1"/>
+    <col min="12" max="12" width="70.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="5" t="s">
+    </row>
+    <row r="4" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L2" s="5" t="s">
+    </row>
+    <row r="5" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="B5" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B6" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
improvements in collection design. glossary
</commit_message>
<xml_diff>
--- a/Assets/Cards/Cards.xlsx
+++ b/Assets/Cards/Cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BBproj\LuckyThicket\Assets\Cards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\LuckyThicket\Assets\Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045877F7-EA34-4FAD-A02B-AA3D5DF50AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD466ABA-5268-43FE-AAF5-A2021F5C57EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Magpies" sheetId="1" r:id="rId1"/>
@@ -96,9 +96,6 @@
     <t>Сорока-болтунья</t>
   </si>
   <si>
-    <t>Free Select Magpie Spawn Beaver Occupied Select Magpie Convert</t>
-  </si>
-  <si>
     <t>Сорока-таксист</t>
   </si>
   <si>
@@ -306,18 +303,9 @@
     <t>Free Select Magpie Spawn Obstacle Occupied Select Unlock</t>
   </si>
   <si>
-    <t>Free Select Magpie Spawn Free Random Await Magpie Spawn</t>
-  </si>
-  <si>
-    <t>Free Select Beaver Spawn Adjacent Free Select Await Beaver Spawn Adjacent Free Select Await Beaver Spawn</t>
-  </si>
-  <si>
     <t>Free Select Beaver Spawn Playable Occupied Select ShiftAnchor NExisting Select Build Drag</t>
   </si>
   <si>
-    <t>Free Select Beaver Spawn Adjacent Free Select Temp Beaver Spawn Adjacent Free Select Temp Beaver Spawn</t>
-  </si>
-  <si>
     <t>Free Select Magpie Spawn Opponent Hand Discard</t>
   </si>
   <si>
@@ -342,21 +330,12 @@
     <t>Бобёр-бармен</t>
   </si>
   <si>
-    <t>Ожидайте двух бобров на смежных клетках.</t>
-  </si>
-  <si>
-    <t>Ожидайте сорочонка на случайной клетке.</t>
-  </si>
-  <si>
     <t>Создайте трёх сорочат на краю поля.</t>
   </si>
   <si>
     <t>Вы уничтожаете случайную клетку (вместе с отрядом).</t>
   </si>
   <si>
-    <t>Вы берете случайную карту из сброса.</t>
-  </si>
-  <si>
     <t>Уничтожьте свободную клетку.</t>
   </si>
   <si>
@@ -378,15 +357,9 @@
     <t>Free Select Magpie Spawn Player Deck Draw</t>
   </si>
   <si>
-    <t>Free Select Magpie Spawn Player Deck Draw Draw Draw Draw Also Player Hand Discard Discard Discard</t>
-  </si>
-  <si>
     <t>Free Select Magpie Spawn Player Deck Draw Adjacent Free Select Destroy</t>
   </si>
   <si>
-    <t>Free Select Magpie Spawn Playable Occupied Select Kill Playable Occupied Adjacent Count Player Deck Draw</t>
-  </si>
-  <si>
     <t>Free Select Magpie Spawn Player Deck Draw Draw Draw Draw</t>
   </si>
   <si>
@@ -417,21 +390,12 @@
     <t>Free Select Magpie Spawn Obstacle Occupied Select Unlock Magpie Spawn</t>
   </si>
   <si>
-    <t>Возьмите 4 карты, а затем сбросьте 3.</t>
-  </si>
-  <si>
     <t>Разблокируйте клетку.</t>
   </si>
   <si>
     <t>Заблокируйте две клетки.</t>
   </si>
   <si>
-    <t>Противник сбрасывает карту.</t>
-  </si>
-  <si>
-    <t>Обратите бобра в сороку.</t>
-  </si>
-  <si>
     <t>Дважды передвиньте сороку.</t>
   </si>
   <si>
@@ -441,12 +405,6 @@
     <t>Возьмите карту и уничтожьте соседнюю свободную клетку.</t>
   </si>
   <si>
-    <t>Поменяйте фракцию смежного отряда.</t>
-  </si>
-  <si>
-    <t>Уничтожьте отряд и возьмите карту за каждый смежный с ним.</t>
-  </si>
-  <si>
     <t>Уничтожьте двух случайных бобров.</t>
   </si>
   <si>
@@ -471,9 +429,6 @@
     <t>Заблокируйте клетку.</t>
   </si>
   <si>
-    <t>Сбросьте две карты и уничтожьте сороку.</t>
-  </si>
-  <si>
     <t>Выберите отряд. Создайте клетку и переместите на неё выбранный отряд.</t>
   </si>
   <si>
@@ -495,18 +450,12 @@
     <t>Вы с противником берёте по две карты.</t>
   </si>
   <si>
-    <t>Если вы не выполняли задач, два случайных отряда меняют фракцию.</t>
-  </si>
-  <si>
     <t>Уничтожьте случайного бобра и двух сорок.</t>
   </si>
   <si>
     <t>Создайте бобра на краю поля и уничтожьте сороку на краю поля.</t>
   </si>
   <si>
-    <t>Создайте двух бобров на смежных клетках. На следующем ходу отряды в этих клетках погибнут.</t>
-  </si>
-  <si>
     <t>Free Select Beaver Spawn Adjacent Magpie Occupied Select Kill</t>
   </si>
   <si>
@@ -516,32 +465,75 @@
     <t>Free Select Magpie Spawn Magpie Occupied Select ShiftAnchor Adjacent Free Select Drag ShiftAnchor Adjacent Free Select Drag</t>
   </si>
   <si>
-    <t xml:space="preserve">Free Select Magpie Spawn Beaver Occupied Adjacent Select Kill Also NExisting Random Build </t>
-  </si>
-  <si>
-    <t>Уничтожьте бобра по соседству и постройте клетку в случайном месте.</t>
-  </si>
-  <si>
-    <t>Free Select Beaver Spawn Completed Zero Playable Occupied Inc Inc Convert</t>
+    <t>Сбросьте две случайные карты и уничтожьте сороку.</t>
+  </si>
+  <si>
+    <t>Противник сбрасывает случайную карту.</t>
+  </si>
+  <si>
+    <t>Создайте бобра на смежной клетке, а затем ещё одного в случайном месте.</t>
+  </si>
+  <si>
+    <t>Free Select Beaver Spawn Adjacent Free Select Beaver Spawn Free Random Beaver Spawn</t>
+  </si>
+  <si>
+    <t>Оттолкните все отряды по соседству и уничтожьте сороку.</t>
+  </si>
+  <si>
+    <t>Free Select Beaver Spawn Playable Occupied Adjacent All Push Magpie Occupied Select Kill</t>
+  </si>
+  <si>
+    <t>Заблокируйте две клетки вокруг и обратите сороку в бобра.</t>
+  </si>
+  <si>
+    <t>Free Select Beaver Spawn Free Surrounding Select Lock Free Surrounding Select Lock Magpie Occupied Select Beaver Convert</t>
+  </si>
+  <si>
+    <t>Создайте сорочонка на случайной клетке.</t>
+  </si>
+  <si>
+    <t>Free Select Magpie Spawn Free Random Magpie Spawn</t>
+  </si>
+  <si>
+    <t>Вы берёте случайную карту из сброса.</t>
+  </si>
+  <si>
+    <t>Возьмите 3 карты, а затем сбросьте 2.</t>
+  </si>
+  <si>
+    <t>Передвиньте двух сорок и заблокируйте клетку.</t>
+  </si>
+  <si>
+    <t>Обратите отряд.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Возьмите две случайные карты из руки противника. </t>
+  </si>
+  <si>
+    <t>Free Select Magpie Spawn Opponent Hand Draw Draw</t>
+  </si>
+  <si>
+    <t>Free Select Magpie Spawn Magpie Occupied Select ShiftAnchor Free Adjacent Select Drag Also Magpie Occupied Select ShiftAnchor Free Adjacent Select Drag Also Free Select Lock</t>
+  </si>
+  <si>
+    <t>Обратите случайного бобра.</t>
+  </si>
+  <si>
+    <t>Free Select Magpie Spawn Beaver Occupied Random Invert</t>
+  </si>
+  <si>
+    <t>Free Select Magpie Spawn Player Deck Draw Draw Draw Also Player Hand Discard Discard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -685,45 +677,45 @@
   </cellStyleXfs>
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -945,25 +937,25 @@
   </sheetPr>
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.08984375" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
     <col min="3" max="3" width="75" customWidth="1"/>
-    <col min="5" max="5" width="99.36328125" customWidth="1"/>
+    <col min="5" max="5" width="99.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -971,7 +963,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D2" s="11">
         <v>0</v>
@@ -980,7 +972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
@@ -988,7 +980,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D3" s="11">
         <v>1</v>
@@ -997,7 +989,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -1005,16 +997,16 @@
         <v>4</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>103</v>
+        <v>151</v>
       </c>
       <c r="D4" s="11">
         <v>2</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>7</v>
       </c>
@@ -1022,23 +1014,23 @@
         <v>4</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>106</v>
+        <v>153</v>
       </c>
       <c r="D5" s="11">
         <v>3</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="11">
         <v>4</v>
       </c>
@@ -1046,7 +1038,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>10</v>
       </c>
@@ -1054,7 +1046,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D7" s="11">
         <v>5</v>
@@ -1063,7 +1055,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>12</v>
       </c>
@@ -1071,7 +1063,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D8" s="11">
         <v>6</v>
@@ -1080,7 +1072,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>14</v>
       </c>
@@ -1088,24 +1080,24 @@
         <v>4</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D9" s="11">
         <v>7</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D10" s="11">
         <v>8</v>
@@ -1114,15 +1106,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D11" s="11">
         <v>9</v>
@@ -1131,49 +1123,49 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="28" t="s">
-        <v>127</v>
+      <c r="C12" s="32" t="s">
+        <v>154</v>
       </c>
       <c r="D12" s="11">
         <v>10</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="28" t="s">
-        <v>128</v>
+      <c r="C13" s="27" t="s">
+        <v>118</v>
       </c>
       <c r="D13" s="11">
         <v>11</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="28" t="s">
-        <v>129</v>
+      <c r="C14" s="27" t="s">
+        <v>119</v>
       </c>
       <c r="D14" s="11">
         <v>12</v>
@@ -1182,24 +1174,24 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>130</v>
+      <c r="C15" s="18" t="s">
+        <v>144</v>
       </c>
       <c r="D15" s="11">
         <v>13</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>23</v>
       </c>
@@ -1207,115 +1199,115 @@
         <v>20</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>131</v>
+        <v>160</v>
       </c>
       <c r="D16" s="11">
         <v>14</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="32" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
-        <v>25</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="D17" s="11">
         <v>15</v>
       </c>
-      <c r="E17" s="30" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="28" t="s">
-        <v>133</v>
+      <c r="C18" s="27" t="s">
+        <v>121</v>
       </c>
       <c r="D18" s="11">
         <v>16</v>
       </c>
       <c r="E18" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
-        <v>28</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="31" t="s">
-        <v>161</v>
+      <c r="C19" s="32" t="s">
+        <v>155</v>
       </c>
       <c r="D19" s="11">
         <v>17</v>
       </c>
-      <c r="E19" s="31" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="32" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="28" t="s">
-        <v>134</v>
+      <c r="C20" s="32" t="s">
+        <v>122</v>
       </c>
       <c r="D20" s="11">
         <v>18</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D21" s="11">
         <v>19</v>
       </c>
-      <c r="E21" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>123</v>
+        <v>31</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>114</v>
       </c>
       <c r="D22" s="11">
         <v>20</v>
       </c>
-      <c r="E22" s="28" t="s">
-        <v>124</v>
+      <c r="E22" s="27" t="s">
+        <v>115</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -1339,72 +1331,72 @@
       <c r="Y22" s="6"/>
       <c r="Z22" s="6"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>135</v>
+      <c r="C23" s="30" t="s">
+        <v>156</v>
       </c>
       <c r="D23" s="11">
         <v>21</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="D24" s="11">
         <v>22</v>
       </c>
-      <c r="E24" s="11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="32" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>137</v>
+        <v>31</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>123</v>
       </c>
       <c r="D25" s="11">
         <v>23</v>
       </c>
       <c r="E25" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
-        <v>38</v>
-      </c>
       <c r="B26" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>138</v>
+        <v>31</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>124</v>
       </c>
       <c r="D26" s="11">
         <v>24</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1423,244 +1415,244 @@
   </sheetPr>
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.453125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" style="8"/>
-    <col min="3" max="3" width="80.6328125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" style="8"/>
-    <col min="5" max="5" width="108.08984375" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="12.6328125" style="8"/>
+    <col min="1" max="1" width="19.44140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="8"/>
+    <col min="3" max="3" width="80.6640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="8"/>
+    <col min="5" max="5" width="108.109375" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="12.6640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
     </row>
-    <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="28" t="s">
-        <v>139</v>
+      <c r="C2" s="27" t="s">
+        <v>125</v>
       </c>
       <c r="D2" s="11">
         <v>25</v>
       </c>
       <c r="E2" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" ht="14" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>41</v>
-      </c>
       <c r="B3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="28" t="s">
-        <v>140</v>
+      <c r="C3" s="27" t="s">
+        <v>126</v>
       </c>
       <c r="D3" s="11">
         <v>26</v>
       </c>
       <c r="E3" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" ht="14" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>43</v>
-      </c>
       <c r="B4" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D4" s="11">
         <v>27</v>
       </c>
       <c r="E4" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" ht="14" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>45</v>
-      </c>
       <c r="B5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="11">
         <v>28</v>
       </c>
       <c r="E5" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" ht="14" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
-        <v>47</v>
-      </c>
       <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="28" t="s">
-        <v>109</v>
+      <c r="C6" s="27" t="s">
+        <v>102</v>
       </c>
       <c r="D6" s="11">
         <v>29</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="28" t="s">
-        <v>141</v>
+      <c r="C7" s="27" t="s">
+        <v>127</v>
       </c>
       <c r="D7" s="11">
         <v>30</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="28" t="s">
-        <v>142</v>
+      <c r="C8" s="27" t="s">
+        <v>128</v>
       </c>
       <c r="D8" s="11">
         <v>31</v>
       </c>
       <c r="E8" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" ht="14" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>51</v>
-      </c>
       <c r="B9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="28" t="s">
-        <v>143</v>
+      <c r="C9" s="27" t="s">
+        <v>129</v>
       </c>
       <c r="D9" s="11">
         <v>32</v>
       </c>
       <c r="E9" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" ht="14" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>53</v>
-      </c>
       <c r="B10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="28" t="s">
-        <v>107</v>
+      <c r="C10" s="27" t="s">
+        <v>100</v>
       </c>
       <c r="D10" s="11">
         <v>33</v>
       </c>
       <c r="E10" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" ht="14" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
-        <v>55</v>
-      </c>
       <c r="B11" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="27" t="s">
-        <v>130</v>
+      <c r="C11" s="30" t="s">
+        <v>144</v>
       </c>
       <c r="D11" s="14">
         <v>34</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="28" t="s">
-        <v>144</v>
+      <c r="C12" s="27" t="s">
+        <v>130</v>
       </c>
       <c r="D12" s="11">
         <v>35</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>145</v>
+      <c r="C13" s="30" t="s">
+        <v>143</v>
       </c>
       <c r="D13" s="14">
         <v>36</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="D14" s="20">
+      <c r="C14" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" s="19">
         <v>37</v>
       </c>
-      <c r="E14" s="24" t="s">
-        <v>92</v>
+      <c r="E14" s="23" t="s">
+        <v>89</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="7"/>
@@ -1684,123 +1676,123 @@
       <c r="Y14" s="7"/>
       <c r="Z14" s="7"/>
     </row>
-    <row r="15" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="D15" s="14">
         <v>38</v>
       </c>
-      <c r="E15" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+      <c r="E15" s="31" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>147</v>
+      <c r="C16" s="32" t="s">
+        <v>132</v>
       </c>
       <c r="D16" s="11">
         <v>39</v>
       </c>
-      <c r="E16" s="29" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+      <c r="E16" s="28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="29" t="s">
-        <v>148</v>
+      <c r="C17" s="28" t="s">
+        <v>133</v>
       </c>
       <c r="D17" s="11">
         <v>40</v>
       </c>
-      <c r="E17" s="29" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+      <c r="E17" s="28" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="28" t="s">
-        <v>149</v>
+      <c r="C18" s="27" t="s">
+        <v>134</v>
       </c>
       <c r="D18" s="11">
         <v>41</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="28" t="s">
-        <v>150</v>
+      <c r="C19" s="27" t="s">
+        <v>135</v>
       </c>
       <c r="D19" s="11">
         <v>42</v>
       </c>
       <c r="E19" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" ht="14" x14ac:dyDescent="0.3">
-      <c r="A20" s="11" t="s">
-        <v>64</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="28" t="s">
-        <v>151</v>
+      <c r="C20" s="27" t="s">
+        <v>136</v>
       </c>
       <c r="D20" s="11">
         <v>43</v>
       </c>
       <c r="E20" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" ht="14" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="D21" s="25">
+      <c r="C21" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="24">
         <v>44</v>
       </c>
-      <c r="E21" s="26" t="s">
-        <v>122</v>
+      <c r="E21" s="25" t="s">
+        <v>113</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -1824,89 +1816,89 @@
       <c r="Y21" s="7"/>
       <c r="Z21" s="7"/>
     </row>
-    <row r="22" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D22" s="14">
         <v>45</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" ht="14" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="19">
+        <v>46</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="20">
-        <v>46</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" ht="14" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
-        <v>69</v>
-      </c>
       <c r="B24" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>154</v>
+        <v>31</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>138</v>
       </c>
       <c r="D24" s="11">
         <v>47</v>
       </c>
       <c r="E24" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="25" spans="1:26" ht="14" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
-        <v>71</v>
-      </c>
       <c r="B25" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>155</v>
+        <v>31</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>139</v>
       </c>
       <c r="D25" s="11">
         <v>48</v>
       </c>
       <c r="E25" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="26" spans="1:26" ht="14" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
-        <v>73</v>
-      </c>
       <c r="B26" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>102</v>
+        <v>31</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>149</v>
       </c>
       <c r="D26" s="14">
         <v>49</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>91</v>
+      <c r="E26" s="32" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1923,77 +1915,77 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.08984375" customWidth="1"/>
-    <col min="6" max="6" width="56.81640625" customWidth="1"/>
+    <col min="1" max="1" width="52.109375" customWidth="1"/>
+    <col min="6" max="6" width="56.77734375" customWidth="1"/>
     <col min="9" max="9" width="57" customWidth="1"/>
-    <col min="12" max="12" width="70.6328125" customWidth="1"/>
+    <col min="12" max="12" width="70.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="L2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="B5" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>

</xml_diff>